<commit_message>
updated IP after experimental DDS-only build
This restores "design intent" following an experimental build
</commit_message>
<xml_diff>
--- a/FPGA/documentation/dds phase word calc.xlsx
+++ b/FPGA/documentation/dds phase word calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xilinxdesigns\Saturn\FPGA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D4128D-74F5-47F7-B615-2BBCEAD81DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5F236C-2156-4272-979D-040FBF6686A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1095" windowWidth="28620" windowHeight="19785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="10635" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -290,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -432,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,7 +443,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>1.7</v>
+        <v>51.5</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -498,7 +498,7 @@
       </c>
       <c r="B9">
         <f>(B7/B3)*2^B4</f>
-        <v>59419306.666666664</v>
+        <v>1800055466.6666667</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
       </c>
       <c r="B10" t="str">
         <f>DEC2HEX(B9,8)</f>
-        <v>038AAAAA</v>
+        <v>6B4AAAAA</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>

</xml_diff>